<commit_message>
added graphs with distributions
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -55,13 +55,13 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -93,16 +93,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -418,18 +415,18 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -587,22 +584,70 @@
       <c r="D11" s="4">
         <v>291</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="4">
         <v>442</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="4">
         <v>569</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
-      <c r="A12" s="4">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+      <c r="A12" s="3">
         <v>69</v>
       </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
+      <c r="A13" s="4">
+        <v>67</v>
+      </c>
+      <c r="B13" s="4">
+        <v>63</v>
+      </c>
+      <c r="C13" s="4">
+        <v>224</v>
+      </c>
+      <c r="D13" s="4">
+        <v>227</v>
+      </c>
+      <c r="E13" s="3">
+        <v>402</v>
+      </c>
+      <c r="F13" s="3">
+        <v>502</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+      <c r="A14" s="3">
+        <v>81</v>
+      </c>
+      <c r="B14" s="3">
+        <v>72</v>
+      </c>
+      <c r="C14" s="3">
+        <v>263</v>
+      </c>
+      <c r="D14" s="3">
+        <v>292</v>
+      </c>
+      <c r="E14" s="3">
+        <v>428</v>
+      </c>
+      <c r="F14" s="3">
+        <v>541</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>